<commit_message>
fill 200 to 235
</commit_message>
<xml_diff>
--- a/splited_sound_with_noise/splited_sound_with_noisesplited_sound_with_noise .xlsx
+++ b/splited_sound_with_noise/splited_sound_with_noisesplited_sound_with_noise .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0 project\megacom\speech\splited_sound_with_noise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69256EB-9DCA-4FAA-9ABB-4832375C5A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FDE9AD-A1B1-4D28-AC3E-3CD9D3C6CD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="2610" windowWidth="13335" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="1395" windowWidth="17700" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="1954">
   <si>
     <t>audio</t>
   </si>
@@ -5823,6 +5823,78 @@
   </si>
   <si>
     <t>جان بله من هر موقع خودم تو تمیرگایم گفتم  تموم بشه میام زود میام</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * اگه قسمت گردنش باشه اشکال نداره</t>
+  </si>
+  <si>
+    <t xml:space="preserve">به سجاد انتقال بده روز چند بارم زنگ زدم گوشیش جواب نداد </t>
+  </si>
+  <si>
+    <t xml:space="preserve">بعد یه مرغ کاملم تیکه شده هم میخاستم هشت تیکه </t>
+  </si>
+  <si>
+    <t>ساعت هشت شب یادداشت کردم براتون  بعد *</t>
+  </si>
+  <si>
+    <t>خب عع کوچیک ترین رونامون امروز کلا رونا درشت بوده کوچیک ترین رون  همون سه و هفصد هشصد هست در کمترین حالت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* میخاید اصن هرموقع حاظر شد بیاین ببرین </t>
+  </si>
+  <si>
+    <t>شنسه عع چیز به صورت استیکی برش خورده  عع شنسل عع بی خطه بدون استخونه و پوستشم گرفته شده دو کیلو اره شنسل</t>
+  </si>
+  <si>
+    <t>خ م دوازده دیگه دس شما درد نکنه ممنون خدافظ خدا</t>
+  </si>
+  <si>
+    <t>بله حاله شما خوبه خسته نباشید ممنونم سلامت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">خیلی خب باشه پس منم پس  میام رون و سینه میگیرم اونجوری بهتره </t>
+  </si>
+  <si>
+    <t>چش یکو دویستش خب گوساله باشه هشصد گرمش گوسفندی باشه</t>
+  </si>
+  <si>
+    <t>در خدمتتون آقایی هستیم سلامت باشید ممنونم مرسی قربان شما  خدانگه دار * *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سلام  سلام فقط یه ساعت میتونید اعلام کنید اگه نیومدید من بعدش بفروشم </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نه با من همیشه میام خدمتتون رون رونی که میگیرم مایه قسمت ماهیچش رو </t>
+  </si>
+  <si>
+    <t xml:space="preserve">عع سلام جناب ترکمی خوبین حال شما خوبه قربونت مرسی </t>
+  </si>
+  <si>
+    <t>خیلی مچکرم ساعت یک خدمتتون میرسم من  در خدمتیم خدانگه دار</t>
+  </si>
+  <si>
+    <t>من نازام برام یه مغز رون خوب میچینی نگه داری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مثلا بوقلمون چرخ کرده و نمیدونم اره </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نه بالای دو کیلو نمیخاما یکو هشصد نه نه  یکو نهصد </t>
+  </si>
+  <si>
+    <t>شما فردا تشریف بیارید هر زمان که شقش کنم باهام مو با شما تماس میگیریم بیاین ببرین</t>
+  </si>
+  <si>
+    <t>پس اطلاع بدین ببخشین ما دنبه رو نمیتونیم بیایم ببریم سلامت باشین بازم ببخشین خواهش میکنم خدانگه دار شما</t>
+  </si>
+  <si>
+    <t>خب خب هشت عددش پوستشو باید دو تیکه بشه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سمت ظهر شلوغه الانم برقا قطعه واسه همون گفتم همون بیاید راحت تره </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نه دیگه اون یدونه لازم نیس فقط یدونه برام ب ععم فاکتور کنید </t>
   </si>
 </sst>
 </file>
@@ -6240,15 +6312,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1843"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A228" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B236" sqref="B236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="67.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8401,6 +8473,9 @@
         <f>HYPERLINK("1739962300_5_SPK_0_20250215_v2.1739612952.2265166.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C210" s="1" t="s">
+        <v>1930</v>
+      </c>
       <c r="F210" t="s">
         <v>1853</v>
       </c>
@@ -8413,14 +8488,20 @@
         <f>HYPERLINK("1739962543_4_SPK_1_20250216_v2.1739698445.2310537.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C211" s="1" t="s">
+        <v>1855</v>
+      </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B212" s="6" t="str">
+      <c r="B212" s="7" t="str">
         <f>HYPERLINK("1739962352_6_SPK_1_20250213_v2.1739441507.2208843.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>1931</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -8431,6 +8512,9 @@
         <f>HYPERLINK("1739962948_10_SPK_1_20250217_v2.1739802175.2383421.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C213" s="1" t="s">
+        <v>1932</v>
+      </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
@@ -8440,23 +8524,32 @@
         <f>HYPERLINK("1739961624_12_SPK_1_20250213_v2.1739437852.2203015.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C214" s="1" t="s">
+        <v>1933</v>
+      </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B215" s="6" t="str">
+      <c r="B215" s="7" t="str">
         <f>HYPERLINK("1739962517_3_SPK_1_20250217_v2.1739793977.2374162.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>1934</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B216" s="6" t="str">
+      <c r="B216" s="7" t="str">
         <f>HYPERLINK("1739962675_3_SPK_1_20250218_v2.1739864093.2431257.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>1935</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
@@ -8467,6 +8560,9 @@
         <f>HYPERLINK("1739962326_3_SPK_1_20250215_v2.1739632205.2283760.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C217" s="1" t="s">
+        <v>1936</v>
+      </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
@@ -8476,6 +8572,9 @@
         <f>HYPERLINK("1739962832_0_SPK_0_20250216_v2.1739723024.2340422.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C218" s="1" t="s">
+        <v>1855</v>
+      </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
@@ -8485,6 +8584,9 @@
         <f>HYPERLINK("1739962624_4_SPK_1_20250216_v2.1739686481.2297600.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C219" s="1" t="s">
+        <v>1937</v>
+      </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
@@ -8494,14 +8596,20 @@
         <f>HYPERLINK("1739962276_0_SPK_1_20250217_v2.1739800568.2381656.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C220" s="1" t="s">
+        <v>1938</v>
+      </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B221" s="6" t="str">
+      <c r="B221" s="7" t="str">
         <f>HYPERLINK("1739962868_8_SPK_1_20250215_v2.1739614231.2265805.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>1939</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -8512,6 +8620,9 @@
         <f>HYPERLINK("1739962517_5_SPK_0_20250217_v2.1739793977.2374162.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C222" s="1" t="s">
+        <v>1940</v>
+      </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
@@ -8521,6 +8632,9 @@
         <f>HYPERLINK("1739962266_18_SPK_0_20250215_v2.1739600840.2256930.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C223" s="1" t="s">
+        <v>1941</v>
+      </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
@@ -8530,8 +8644,11 @@
         <f>HYPERLINK("1739962180_1_SPK_1_20250216_v2.1739702235.2316694.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C224" s="1" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>226</v>
       </c>
@@ -8539,17 +8656,23 @@
         <f>HYPERLINK("1739962998_9_SPK_0_20250216_v2.1739697766.2309766.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C225" s="1" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B226" s="6" t="str">
+      <c r="B226" s="7" t="str">
         <f>HYPERLINK("1739962486_5_SPK_1_20250215_v2.1739627574.2281608.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C226" s="1" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
         <v>228</v>
       </c>
@@ -8557,17 +8680,23 @@
         <f>HYPERLINK("1739962293_15_SPK_0_20250218_v2.1739858897.2424782.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C227" s="1" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B228" s="6" t="str">
+      <c r="B228" s="7" t="str">
         <f>HYPERLINK("1739961707_2_SPK_0_20250213_v2.1739437852.2203015.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C228" s="1" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
         <v>230</v>
       </c>
@@ -8575,8 +8704,11 @@
         <f>HYPERLINK("1739962861_32_SPK_1_20250216_v2.1739695895.2308017.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C229" s="1" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
         <v>231</v>
       </c>
@@ -8584,17 +8716,23 @@
         <f>HYPERLINK("1739962826_8_SPK_0_20250215_v2.1739596848.2256007.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C230" s="1" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B231" s="6" t="str">
+      <c r="B231" s="7" t="str">
         <f>HYPERLINK("1739962597_10_SPK_1_20250215_v2.1739624662.2279909.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C231" s="1" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
         <v>233</v>
       </c>
@@ -8602,8 +8740,11 @@
         <f>HYPERLINK("1739961708_3_SPK_0_20250213_v2.1739437852.2203015.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C232" s="1" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
         <v>234</v>
       </c>
@@ -8611,8 +8752,11 @@
         <f>HYPERLINK("1739962642_6_SPK_1_20250218_v2.1739864664.2432073.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C233" s="1" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
         <v>235</v>
       </c>
@@ -8620,8 +8764,11 @@
         <f>HYPERLINK("1739962161_16_SPK_0_20250215_v2.1739603840.2258967.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C234" s="1" t="s">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
         <v>236</v>
       </c>
@@ -8629,8 +8776,11 @@
         <f>HYPERLINK("1739962955_11_SPK_1_20250213_v2.1739439090.2205291.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C235" s="1" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
         <v>237</v>
       </c>
@@ -8639,7 +8789,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
         <v>238</v>
       </c>
@@ -8648,7 +8798,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
         <v>239</v>
       </c>
@@ -8657,7 +8807,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
         <v>240</v>
       </c>
@@ -8666,7 +8816,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
         <v>241</v>
       </c>

</xml_diff>